<commit_message>
Started adding functionalities for stopwatch, not working just yet
</commit_message>
<xml_diff>
--- a/WorkingProject/TouchGFX/assets/texts/texts.xlsx
+++ b/WorkingProject/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7417" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8011" uniqueCount="237">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -773,6 +773,60 @@
   </si>
   <si>
     <t xml:space="preserve">Cell Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(accel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start/Stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99:99.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_12</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2306,7 @@
         <v>105</v>
       </c>
       <c r="D11">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -2274,7 +2328,7 @@
         <v>105</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -2352,6 +2406,92 @@
       <c r="H15"/>
       <c r="I15"/>
       <c r="J15"/>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
     </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -2545,7 +2685,7 @@
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12">
@@ -2579,7 +2719,7 @@
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14">
@@ -2587,7 +2727,7 @@
         <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>219</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -2596,12 +2736,12 @@
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
@@ -2613,32 +2753,32 @@
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
         <v>51</v>
@@ -2647,15 +2787,15 @@
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -2664,32 +2804,32 @@
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -2698,15 +2838,15 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>214</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -2715,15 +2855,15 @@
         <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>214</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
@@ -2732,32 +2872,32 @@
         <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="C23" t="s">
-        <v>210</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -2766,15 +2906,15 @@
         <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>216</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C25" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
@@ -2783,7 +2923,58 @@
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>218</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>230</v>
+      </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6-9 introducing Arduino CAN Shield Functions to STM Libraries
</commit_message>
<xml_diff>
--- a/WorkingProject/TouchGFX/assets/texts/texts.xlsx
+++ b/WorkingProject/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9216" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10686" uniqueCount="267">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -912,6 +912,27 @@
   </si>
   <si>
     <t xml:space="preserve">75%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOLD FOOT ON BRAKE!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START CAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Engine</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2378,7 @@
         <v>105</v>
       </c>
       <c r="D10">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -2619,6 +2640,48 @@
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
     </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -2687,7 +2750,7 @@
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>260</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -2701,7 +2764,7 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>261</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
@@ -2710,7 +2773,7 @@
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
@@ -2902,10 +2965,10 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
-        <v>220</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -2914,15 +2977,15 @@
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>214</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -2931,15 +2994,15 @@
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C19" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -2948,32 +3011,32 @@
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C21" t="s">
-        <v>214</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -2982,66 +3045,66 @@
         <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>218</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>220</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>225</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>227</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>138</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C24" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C25" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D25" t="s">
         <v>51</v>
@@ -3050,15 +3113,15 @@
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C26" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
@@ -3067,15 +3130,15 @@
         <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D27" t="s">
         <v>51</v>
@@ -3084,12 +3147,12 @@
         <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C28" t="s">
         <v>237</v>
@@ -3101,46 +3164,46 @@
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C30" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
         <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s">
         <v>238</v>
@@ -3152,15 +3215,15 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
         <v>46</v>
@@ -3169,15 +3232,15 @@
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>248</v>
+        <v>193</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -3186,7 +3249,7 @@
         <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>249</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginning of SPI_Transfer function in SPI.h
</commit_message>
<xml_diff>
--- a/WorkingProject/TouchGFX/assets/texts/texts.xlsx
+++ b/WorkingProject/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10686" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11957" uniqueCount="284">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -933,6 +933,62 @@
   </si>
   <si>
     <t xml:space="preserve">Start Engine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRADM.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCB_____.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Hold Foot on Brake
+2) Hold Gamecock Logo for 3 SEC to START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Hold Foot on Brake
+2) Hold Gamecock Logo for 3 SEC to START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date &amp; Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charging Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charged Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Hold Foot on Brake
+2) Hold Gamecock Logo for 3 SEC to START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Hold Foot on Brake
+2) Hold Gamecock Logo for 3 SEC to START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Hold Foot on Brake
+2) Hold Gamecock Logo for 3 SEC to START</t>
   </si>
 </sst>
 </file>
@@ -2163,7 +2219,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>267</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -2269,7 +2325,7 @@
         <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>267</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -2375,7 +2431,7 @@
         <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>267</v>
       </c>
       <c r="D10">
         <v>22</v>
@@ -2646,7 +2702,7 @@
         <v>261</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>268</v>
       </c>
       <c r="D22">
         <v>22</v>
@@ -2682,6 +2738,27 @@
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24">
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
     </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -2761,44 +2838,44 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>211</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -2807,83 +2884,83 @@
         <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>237</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>219</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2892,83 +2969,83 @@
         <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>222</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>155</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>100</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -2977,12 +3054,12 @@
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
         <v>214</v>
@@ -2994,49 +3071,49 @@
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>225</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>220</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -3045,29 +3122,29 @@
         <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>138</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C22" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C23" t="s">
         <v>227</v>
@@ -3079,15 +3156,15 @@
         <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C24" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -3096,15 +3173,15 @@
         <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C25" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D25" t="s">
         <v>51</v>
@@ -3113,12 +3190,12 @@
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C26" t="s">
         <v>237</v>
@@ -3130,12 +3207,12 @@
         <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C27" t="s">
         <v>237</v>
@@ -3147,29 +3224,29 @@
         <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C28" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C29" t="s">
         <v>238</v>
@@ -3181,15 +3258,15 @@
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>246</v>
+        <v>193</v>
       </c>
       <c r="C30" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -3198,60 +3275,78 @@
         <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>247</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
+        <v>271</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>249</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>193</v>
+        <v>277</v>
       </c>
       <c r="C33" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
-      </c>
-    </row>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>279</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
UART Round 1 Changes
</commit_message>
<xml_diff>
--- a/WorkingProject/TouchGFX/assets/texts/texts.xlsx
+++ b/WorkingProject/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11957" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12043" uniqueCount="285">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -989,6 +989,9 @@
   <si>
     <t xml:space="preserve">1) Hold Foot on Brake
 2) Hold Gamecock Logo for 3 SEC to START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN Message Output</t>
   </si>
 </sst>
 </file>
@@ -2231,9 +2234,7 @@
         <v>17</v>
       </c>
       <c r="G4"/>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
+      <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
@@ -2607,9 +2608,7 @@
         <v>17</v>
       </c>
       <c r="G17"/>
-      <c r="H17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
@@ -2821,27 +2820,27 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
@@ -2850,502 +2849,54 @@
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>283</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>284</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="s">
-        <v>195</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="s">
-        <v>215</v>
-      </c>
-      <c r="C17" t="s">
-        <v>214</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="s">
-        <v>217</v>
-      </c>
-      <c r="C18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="s">
-        <v>224</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="s">
-        <v>226</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="s">
-        <v>229</v>
-      </c>
-      <c r="C21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C22" t="s">
-        <v>227</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="s">
-        <v>232</v>
-      </c>
-      <c r="C23" t="s">
-        <v>227</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s">
-        <v>234</v>
-      </c>
-      <c r="C24" t="s">
-        <v>236</v>
-      </c>
-      <c r="D24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="s">
-        <v>239</v>
-      </c>
-      <c r="C25" t="s">
-        <v>237</v>
-      </c>
-      <c r="D25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="s">
-        <v>241</v>
-      </c>
-      <c r="C26" t="s">
-        <v>237</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="s">
-        <v>243</v>
-      </c>
-      <c r="C27" t="s">
-        <v>237</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="s">
-        <v>246</v>
-      </c>
-      <c r="C28" t="s">
-        <v>238</v>
-      </c>
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="s">
-        <v>248</v>
-      </c>
-      <c r="C29" t="s">
-        <v>238</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="s">
-        <v>193</v>
-      </c>
-      <c r="C30" t="s">
-        <v>220</v>
-      </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" t="s">
-        <v>274</v>
-      </c>
-      <c r="C31" t="s">
-        <v>271</v>
-      </c>
-      <c r="D31" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="s">
-        <v>275</v>
-      </c>
-      <c r="C32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="s">
-        <v>277</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="s">
-        <v>279</v>
-      </c>
-      <c r="C34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" t="s">
-        <v>280</v>
-      </c>
-    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
     <row r="35"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>